<commit_message>
investing.com Calculator functionality test
</commit_message>
<xml_diff>
--- a/com.investing/src/test/resources/test_data.xlsx
+++ b/com.investing/src/test/resources/test_data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vikto\IdeaProjects\SeleniumBootcamp\com.investing\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2C22F6F-4AEE-4CFB-ACC1-2FA025C93590}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14EF8081-60EC-4545-811C-ADB1B8EED605}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="924" yWindow="2040" windowWidth="17280" windowHeight="8880" xr2:uid="{3F55D5A8-7241-4387-A619-14456C32AEF6}"/>
+    <workbookView xWindow="2748" yWindow="1908" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{3F55D5A8-7241-4387-A619-14456C32AEF6}"/>
   </bookViews>
   <sheets>
     <sheet name="LogInValidCredentials" sheetId="1" r:id="rId1"/>
+    <sheet name="CalculatorCurrency" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>iudgdsoug@gmail.com</t>
   </si>
@@ -69,12 +70,27 @@
   </si>
   <si>
     <t>Please enter a valid email address</t>
+  </si>
+  <si>
+    <t>EUR/USD</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>1.06</t>
+  </si>
+  <si>
+    <t>$60</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -113,9 +129,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -433,7 +451,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F90CFB6C-F421-476B-A017-E71FCF3FFB43}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -493,4 +511,37 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4170E66-B8B1-4D98-B3CB-EE3FA373FAB4}">
+  <dimension ref="A2:A5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
investing.com Mortgage Calculator functionality testing
</commit_message>
<xml_diff>
--- a/com.investing/src/test/resources/test_data.xlsx
+++ b/com.investing/src/test/resources/test_data.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vikto\IdeaProjects\SeleniumBootcamp\com.investing\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14EF8081-60EC-4545-811C-ADB1B8EED605}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F23A6DC-C5A1-4215-91FB-8E8B5BDE5DA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2748" yWindow="1908" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{3F55D5A8-7241-4387-A619-14456C32AEF6}"/>
+    <workbookView xWindow="2076" yWindow="1728" windowWidth="17280" windowHeight="8880" activeTab="2" xr2:uid="{3F55D5A8-7241-4387-A619-14456C32AEF6}"/>
   </bookViews>
   <sheets>
     <sheet name="LogInValidCredentials" sheetId="1" r:id="rId1"/>
     <sheet name="CalculatorCurrency" sheetId="2" r:id="rId2"/>
+    <sheet name="MortgageCalculator" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>iudgdsoug@gmail.com</t>
   </si>
@@ -82,6 +83,18 @@
   </si>
   <si>
     <t>$60</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>300000</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>$2,149.29</t>
   </si>
 </sst>
 </file>
@@ -129,11 +142,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -517,7 +531,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4170E66-B8B1-4D98-B3CB-EE3FA373FAB4}">
   <dimension ref="A2:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -544,4 +558,42 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C190DEC6-EE8A-44E6-8CF1-E5A89CCD3AEF}">
+  <dimension ref="A2:A5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>